<commit_message>
imprimir rotas em pdf, fazer as rotas, corrigir erros
</commit_message>
<xml_diff>
--- a/Data/planilha_local.xlsx
+++ b/Data/planilha_local.xlsx
@@ -524,7 +524,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2/10/2024</t>
+          <t>11/4/2024</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -583,7 +583,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>8:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -605,7 +605,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2/10/2024</t>
+          <t>11/4/2024</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -678,7 +678,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2/10/2024</t>
+          <t>11/4/2024</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -755,11 +755,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2/10/2024</t>
+          <t>11/4/2024</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>88075142</v>
+        <v>88070142</v>
       </c>
       <c r="D5" t="n">
         <v>254</v>
@@ -832,7 +832,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2/10/2024</t>
+          <t>11/4/2024</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -909,7 +909,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2/10/2024</t>
+          <t>11/5/2024</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -990,14 +990,14 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2/10/2024</t>
+          <t>11/5/2024</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>88095830</v>
+        <v>88106550</v>
       </c>
       <c r="D8" t="n">
-        <v>23</v>
+        <v>150</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1063,7 +1063,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2/10/2024</t>
+          <t>11/5/2024</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -1136,7 +1136,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2/10/2024</t>
+          <t>11/5/2024</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2/10/2024</t>
+          <t>11/5/2024</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -1294,7 +1294,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2/10/2024</t>
+          <t>11/6/2024</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2/10/2024</t>
+          <t>11/6/2024</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -1448,7 +1448,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2/10/2024</t>
+          <t>11/6/2024</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -1521,7 +1521,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2/10/2024</t>
+          <t>11/6/2024</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -1598,7 +1598,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>3/10/2024</t>
+          <t>11/5/2024</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -1679,7 +1679,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>3/10/2024</t>
+          <t>11/5/2024</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -1752,7 +1752,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3/10/2024</t>
+          <t>11/4/2024</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -1825,7 +1825,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>3/10/2024</t>
+          <t>11/6/2024</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -1898,7 +1898,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3/10/2024</t>
+          <t>11/6/2024</t>
         </is>
       </c>
       <c r="C20" t="n">

</xml_diff>

<commit_message>
o código agora está separando corretamente entre os turnos e gerando os pdfs, porém os pdfs ainda estão sem os dados dos clientes, para visualizar esses dados é preciso entrar em file2.json napasta data
</commit_message>
<xml_diff>
--- a/Data/planilha_local.xlsx
+++ b/Data/planilha_local.xlsx
@@ -956,10 +956,8 @@
       <c r="F6" t="n">
         <v>4</v>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>0:00</t>
-        </is>
+      <c r="G6" t="n">
+        <v>35</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -996,10 +994,8 @@
           <t>CASA</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>0:00</t>
-        </is>
+      <c r="O6" t="n">
+        <v>1</v>
       </c>
       <c r="P6" t="inlineStr">
         <is>
@@ -1336,10 +1332,8 @@
       <c r="F10" t="n">
         <v>2</v>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>0:00</t>
-        </is>
+      <c r="G10" t="n">
+        <v>25</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -1376,10 +1370,8 @@
           <t>CASA</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>0:00</t>
-        </is>
+      <c r="O10" t="n">
+        <v>1</v>
       </c>
       <c r="P10" t="inlineStr">
         <is>
@@ -1810,10 +1802,8 @@
       <c r="F15" t="n">
         <v>2</v>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>0:00</t>
-        </is>
+      <c r="G15" t="n">
+        <v>40</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -1850,10 +1840,8 @@
           <t>APARTAMENTO</t>
         </is>
       </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>0:00</t>
-        </is>
+      <c r="O15" t="n">
+        <v>4</v>
       </c>
       <c r="P15" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
lógica dos turnos terminada, pdfs e planilhas salvos como retorno, divisão entre caminhões pronto, criação de um arquivo json com os clientes não atendidos pronto, criação de um arquivo pdf e/ou planilha com os clientes não atendidos faltando
</commit_message>
<xml_diff>
--- a/Data/planilha_local.xlsx
+++ b/Data/planilha_local.xlsx
@@ -557,7 +557,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -655,7 +655,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>09/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -749,7 +749,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>09/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -769,7 +769,7 @@
         <v>3</v>
       </c>
       <c r="G4" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -831,7 +831,7 @@
         <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X4" t="n">
         <v>0</v>
@@ -843,7 +843,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -863,7 +863,7 @@
         <v>21</v>
       </c>
       <c r="G5" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -925,7 +925,7 @@
         <v>20</v>
       </c>
       <c r="W5" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X5" t="n">
         <v>0</v>
@@ -937,7 +937,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1031,7 +1031,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>09/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1125,7 +1125,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>08/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1145,7 +1145,7 @@
         <v>21</v>
       </c>
       <c r="G8" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -1207,7 +1207,7 @@
         <v>20</v>
       </c>
       <c r="W8" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X8" t="n">
         <v>0</v>
@@ -1219,7 +1219,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1239,7 +1239,7 @@
         <v>21</v>
       </c>
       <c r="G9" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -1301,7 +1301,7 @@
         <v>20</v>
       </c>
       <c r="W9" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X9" t="n">
         <v>0</v>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1407,7 +1407,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1521,7 +1521,7 @@
         <v>2</v>
       </c>
       <c r="G12" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -1583,7 +1583,7 @@
         <v>20</v>
       </c>
       <c r="W12" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X12" t="n">
         <v>0</v>
@@ -1595,7 +1595,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1615,7 +1615,7 @@
         <v>2</v>
       </c>
       <c r="G13" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -1677,7 +1677,7 @@
         <v>20</v>
       </c>
       <c r="W13" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X13" t="n">
         <v>0</v>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1783,7 +1783,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>09/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1877,7 +1877,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>09/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1897,7 +1897,7 @@
         <v>4</v>
       </c>
       <c r="G16" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -1959,7 +1959,7 @@
         <v>0</v>
       </c>
       <c r="W16" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X16" t="n">
         <v>0</v>
@@ -1971,7 +1971,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1991,7 +1991,7 @@
         <v>2</v>
       </c>
       <c r="G17" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -2053,7 +2053,7 @@
         <v>20</v>
       </c>
       <c r="W17" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X17" t="n">
         <v>0</v>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>09/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -2159,7 +2159,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -2253,7 +2253,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -2273,7 +2273,7 @@
         <v>4</v>
       </c>
       <c r="G20" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -2335,7 +2335,7 @@
         <v>0</v>
       </c>
       <c r="W20" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X20" t="n">
         <v>0</v>
@@ -2347,7 +2347,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -2441,7 +2441,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -2535,7 +2535,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>08/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -2555,7 +2555,7 @@
         <v>4</v>
       </c>
       <c r="G23" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
@@ -2617,7 +2617,7 @@
         <v>0</v>
       </c>
       <c r="W23" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X23" t="n">
         <v>0</v>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -2649,7 +2649,7 @@
         <v>2</v>
       </c>
       <c r="G24" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
@@ -2711,7 +2711,7 @@
         <v>20</v>
       </c>
       <c r="W24" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X24" t="n">
         <v>0</v>
@@ -2723,7 +2723,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>09/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -2911,7 +2911,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -2931,7 +2931,7 @@
         <v>4</v>
       </c>
       <c r="G27" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
@@ -2993,7 +2993,7 @@
         <v>0</v>
       </c>
       <c r="W27" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X27" t="n">
         <v>0</v>
@@ -3005,7 +3005,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -3025,7 +3025,7 @@
         <v>4</v>
       </c>
       <c r="G28" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
@@ -3087,7 +3087,7 @@
         <v>0</v>
       </c>
       <c r="W28" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X28" t="n">
         <v>0</v>
@@ -3099,7 +3099,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -3193,7 +3193,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>09/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -3287,7 +3287,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -3307,7 +3307,7 @@
         <v>4</v>
       </c>
       <c r="G31" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
@@ -3369,7 +3369,7 @@
         <v>0</v>
       </c>
       <c r="W31" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X31" t="n">
         <v>0</v>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -3401,7 +3401,7 @@
         <v>4</v>
       </c>
       <c r="G32" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
@@ -3463,7 +3463,7 @@
         <v>0</v>
       </c>
       <c r="W32" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X32" t="n">
         <v>0</v>
@@ -3475,7 +3475,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>12/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -3569,7 +3569,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>09/11/2024</t>
+          <t>12/11/2024</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -3663,7 +3663,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -3683,7 +3683,7 @@
         <v>4</v>
       </c>
       <c r="G35" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
@@ -3745,7 +3745,7 @@
         <v>0</v>
       </c>
       <c r="W35" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X35" t="n">
         <v>0</v>
@@ -3757,7 +3757,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>09/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -3777,7 +3777,7 @@
         <v>4</v>
       </c>
       <c r="G36" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
@@ -3839,7 +3839,7 @@
         <v>0</v>
       </c>
       <c r="W36" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X36" t="n">
         <v>0</v>
@@ -3851,7 +3851,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>12/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -3945,7 +3945,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>09/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -4039,7 +4039,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -4059,7 +4059,7 @@
         <v>4</v>
       </c>
       <c r="G39" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
@@ -4121,7 +4121,7 @@
         <v>0</v>
       </c>
       <c r="W39" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X39" t="n">
         <v>0</v>
@@ -4133,7 +4133,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -4227,7 +4227,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>09/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -4321,7 +4321,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>09/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -4341,7 +4341,7 @@
         <v>4</v>
       </c>
       <c r="G42" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
@@ -4403,7 +4403,7 @@
         <v>0</v>
       </c>
       <c r="W42" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X42" t="n">
         <v>0</v>
@@ -4415,7 +4415,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>09/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -4435,7 +4435,7 @@
         <v>4</v>
       </c>
       <c r="G43" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
@@ -4497,7 +4497,7 @@
         <v>0</v>
       </c>
       <c r="W43" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X43" t="n">
         <v>0</v>
@@ -4509,7 +4509,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -4603,7 +4603,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -4697,7 +4697,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>08/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -4717,7 +4717,7 @@
         <v>2</v>
       </c>
       <c r="G46" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
@@ -4779,7 +4779,7 @@
         <v>20</v>
       </c>
       <c r="W46" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X46" t="n">
         <v>0</v>
@@ -4791,7 +4791,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -4811,7 +4811,7 @@
         <v>2</v>
       </c>
       <c r="G47" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
@@ -4873,7 +4873,7 @@
         <v>20</v>
       </c>
       <c r="W47" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X47" t="n">
         <v>0</v>
@@ -4885,7 +4885,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>12/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -4979,7 +4979,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>12/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -5073,7 +5073,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>09/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -5093,7 +5093,7 @@
         <v>4</v>
       </c>
       <c r="G50" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H50" t="inlineStr">
         <is>
@@ -5155,7 +5155,7 @@
         <v>0</v>
       </c>
       <c r="W50" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X50" t="n">
         <v>0</v>
@@ -5167,7 +5167,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -5187,7 +5187,7 @@
         <v>4</v>
       </c>
       <c r="G51" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
@@ -5249,7 +5249,7 @@
         <v>0</v>
       </c>
       <c r="W51" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X51" t="n">
         <v>0</v>
@@ -5261,7 +5261,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -5355,7 +5355,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>12/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -5449,7 +5449,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -5469,7 +5469,7 @@
         <v>4</v>
       </c>
       <c r="G54" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H54" t="inlineStr">
         <is>
@@ -5531,7 +5531,7 @@
         <v>0</v>
       </c>
       <c r="W54" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X54" t="n">
         <v>0</v>
@@ -5543,7 +5543,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>12/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -5563,7 +5563,7 @@
         <v>4</v>
       </c>
       <c r="G55" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H55" t="inlineStr">
         <is>
@@ -5625,7 +5625,7 @@
         <v>0</v>
       </c>
       <c r="W55" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X55" t="n">
         <v>0</v>
@@ -5637,7 +5637,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>12/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -5731,7 +5731,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -5825,7 +5825,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -5845,7 +5845,7 @@
         <v>2</v>
       </c>
       <c r="G58" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H58" t="inlineStr">
         <is>
@@ -5907,7 +5907,7 @@
         <v>20</v>
       </c>
       <c r="W58" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X58" t="n">
         <v>0</v>
@@ -5919,7 +5919,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>09/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -6013,7 +6013,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>09/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -6107,7 +6107,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -6127,7 +6127,7 @@
         <v>4</v>
       </c>
       <c r="G61" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H61" t="inlineStr">
         <is>
@@ -6189,7 +6189,7 @@
         <v>0</v>
       </c>
       <c r="W61" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X61" t="n">
         <v>0</v>
@@ -6201,7 +6201,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>09/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -6221,7 +6221,7 @@
         <v>4</v>
       </c>
       <c r="G62" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
@@ -6283,7 +6283,7 @@
         <v>0</v>
       </c>
       <c r="W62" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X62" t="n">
         <v>0</v>
@@ -6295,7 +6295,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -6389,7 +6389,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -6483,7 +6483,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>12/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -6503,7 +6503,7 @@
         <v>4</v>
       </c>
       <c r="G65" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H65" t="inlineStr">
         <is>
@@ -6565,7 +6565,7 @@
         <v>0</v>
       </c>
       <c r="W65" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X65" t="n">
         <v>0</v>
@@ -6577,7 +6577,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -6597,7 +6597,7 @@
         <v>4</v>
       </c>
       <c r="G66" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H66" t="inlineStr">
         <is>
@@ -6659,7 +6659,7 @@
         <v>0</v>
       </c>
       <c r="W66" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X66" t="n">
         <v>0</v>
@@ -6671,7 +6671,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -6765,7 +6765,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -6859,7 +6859,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>09/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -6879,7 +6879,7 @@
         <v>2</v>
       </c>
       <c r="G69" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H69" t="inlineStr">
         <is>
@@ -6941,7 +6941,7 @@
         <v>20</v>
       </c>
       <c r="W69" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X69" t="n">
         <v>0</v>
@@ -6953,7 +6953,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -6973,7 +6973,7 @@
         <v>2</v>
       </c>
       <c r="G70" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H70" t="inlineStr">
         <is>
@@ -7035,7 +7035,7 @@
         <v>20</v>
       </c>
       <c r="W70" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X70" t="n">
         <v>0</v>
@@ -7047,7 +7047,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -7141,7 +7141,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -7235,7 +7235,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>09/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -7255,7 +7255,7 @@
         <v>4</v>
       </c>
       <c r="G73" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H73" t="inlineStr">
         <is>
@@ -7317,7 +7317,7 @@
         <v>0</v>
       </c>
       <c r="W73" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X73" t="n">
         <v>0</v>
@@ -7329,7 +7329,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>12/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -7349,7 +7349,7 @@
         <v>4</v>
       </c>
       <c r="G74" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H74" t="inlineStr">
         <is>
@@ -7411,7 +7411,7 @@
         <v>0</v>
       </c>
       <c r="W74" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X74" t="n">
         <v>0</v>
@@ -7423,7 +7423,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>12/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -7517,7 +7517,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -7611,7 +7611,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -7631,7 +7631,7 @@
         <v>2</v>
       </c>
       <c r="G77" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H77" t="inlineStr">
         <is>
@@ -7693,7 +7693,7 @@
         <v>20</v>
       </c>
       <c r="W77" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X77" t="n">
         <v>0</v>
@@ -7705,7 +7705,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -7799,7 +7799,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -7913,7 +7913,7 @@
         <v>2</v>
       </c>
       <c r="G80" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H80" t="inlineStr">
         <is>
@@ -7975,7 +7975,7 @@
         <v>20</v>
       </c>
       <c r="W80" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X80" t="n">
         <v>0</v>
@@ -7987,7 +7987,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>12/11/2024</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -8007,7 +8007,7 @@
         <v>4</v>
       </c>
       <c r="G81" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H81" t="inlineStr">
         <is>
@@ -8069,7 +8069,7 @@
         <v>0</v>
       </c>
       <c r="W81" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X81" t="n">
         <v>0</v>
@@ -8081,7 +8081,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -8175,7 +8175,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -8269,7 +8269,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>09/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -8289,7 +8289,7 @@
         <v>4</v>
       </c>
       <c r="G84" t="n">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="H84" t="inlineStr">
         <is>
@@ -8351,7 +8351,7 @@
         <v>0</v>
       </c>
       <c r="W84" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X84" t="n">
         <v>0</v>
@@ -8363,7 +8363,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -8383,7 +8383,7 @@
         <v>4</v>
       </c>
       <c r="G85" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H85" t="inlineStr">
         <is>
@@ -8445,7 +8445,7 @@
         <v>0</v>
       </c>
       <c r="W85" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X85" t="n">
         <v>0</v>
@@ -8457,7 +8457,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -8551,7 +8551,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -8645,7 +8645,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -8665,7 +8665,7 @@
         <v>4</v>
       </c>
       <c r="G88" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H88" t="inlineStr">
         <is>
@@ -8727,7 +8727,7 @@
         <v>0</v>
       </c>
       <c r="W88" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X88" t="n">
         <v>0</v>
@@ -8739,7 +8739,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -8759,7 +8759,7 @@
         <v>4</v>
       </c>
       <c r="G89" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H89" t="inlineStr">
         <is>
@@ -8821,7 +8821,7 @@
         <v>0</v>
       </c>
       <c r="W89" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X89" t="n">
         <v>0</v>
@@ -8833,7 +8833,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>08/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -8927,7 +8927,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -9019,7 +9019,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>12/11/2024</t>
+          <t>14/11/2024</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -9039,7 +9039,7 @@
         <v>4</v>
       </c>
       <c r="G92" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H92" t="inlineStr">
         <is>
@@ -9099,7 +9099,7 @@
         <v>0</v>
       </c>
       <c r="W92" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X92" t="n">
         <v>0</v>
@@ -9111,7 +9111,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>10/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -9131,7 +9131,7 @@
         <v>4</v>
       </c>
       <c r="G93" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H93" t="inlineStr">
         <is>
@@ -9191,7 +9191,7 @@
         <v>0</v>
       </c>
       <c r="W93" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X93" t="n">
         <v>0</v>
@@ -9203,7 +9203,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>09/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -9295,7 +9295,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>09/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -9387,7 +9387,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>12/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -9407,7 +9407,7 @@
         <v>4</v>
       </c>
       <c r="G96" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H96" t="inlineStr">
         <is>
@@ -9467,7 +9467,7 @@
         <v>0</v>
       </c>
       <c r="W96" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X96" t="n">
         <v>0</v>
@@ -9479,7 +9479,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>09/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -9571,7 +9571,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -9663,7 +9663,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -9683,7 +9683,7 @@
         <v>4</v>
       </c>
       <c r="G99" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H99" t="inlineStr">
         <is>
@@ -9743,7 +9743,7 @@
         <v>0</v>
       </c>
       <c r="W99" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X99" t="n">
         <v>0</v>
@@ -9755,7 +9755,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>11/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -9775,7 +9775,7 @@
         <v>4</v>
       </c>
       <c r="G100" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H100" t="inlineStr">
         <is>
@@ -9835,7 +9835,7 @@
         <v>0</v>
       </c>
       <c r="W100" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="X100" t="n">
         <v>0</v>

</xml_diff>